<commit_message>
Vanilla Quests Expanded - The Generator 오류 수정
#1917
</commit_message>
<xml_diff>
--- a/Data/Vanilla Expanded/Vanilla Quests Expanded - The Generator - 3411401573/1.6/3411401573.xlsx
+++ b/Data/Vanilla Expanded/Vanilla Quests Expanded - The Generator - 3411401573/1.6/3411401573.xlsx
@@ -2887,7 +2887,7 @@
     <t xml:space="preserve">siteThreat-&gt;guarded by [Number] aggressive [AnimalPlural]</t>
   </si>
   <si>
-    <t xml:space="preserve">siteThreat- [Number]마리의 공격적인 [AnimalPlural]의 본거지</t>
+    <t xml:space="preserve">siteThreat-&gt;[Number]마리의 공격적인 [AnimalPlural]의 본거지</t>
   </si>
   <si>
     <t xml:space="preserve">QuestScriptDef+VQE_AbandonedARC.questDescriptionRules.rulesStrings.31</t>
@@ -10210,6 +10210,7 @@
       <color rgb="FF000000"/>
       <name val="나눔고딕"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -10293,19 +10294,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10563,16 +10564,19 @@
   </sheetPr>
   <dimension ref="A1:F911"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A617" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C645" activeCellId="0" sqref="C645"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C219" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F255" activeCellId="0" sqref="F255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.6328125" defaultRowHeight="16.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="76.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="63.93"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="1" width="7.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="60.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="37.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="1" width="7.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>